<commit_message>
fixing large image file commit
</commit_message>
<xml_diff>
--- a/data/data_digitization/rbcm_data/label_data/RBCM-label-entry-template.xlsx
+++ b/data/data_digitization/rbcm_data/label_data/RBCM-label-entry-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/collection_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/rbcm_data/label_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3399440C-D5FC-6A43-8F14-546B3DEE9A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FFD4F-1420-7C45-929B-C186F6EDC624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="10000" windowHeight="16880" xr2:uid="{6B6DF4C7-2696-B14D-857F-7620348251C6}"/>
   </bookViews>
   <sheets>
     <sheet name="RBCM-label-entry-template" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>accessionNum</t>
   </si>
@@ -44,12 +44,6 @@
     <t>recordNum</t>
   </si>
   <si>
-    <t xml:space="preserve">Achillea millefolium </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Achillea millefolium L. </t>
-  </si>
-  <si>
     <t>habitatDescription</t>
   </si>
   <si>
@@ -62,54 +56,113 @@
     <t>Saturna Island</t>
   </si>
   <si>
-    <t>origTaxonName</t>
-  </si>
-  <si>
-    <t>origFullName</t>
-  </si>
-  <si>
-    <t>revName</t>
-  </si>
-  <si>
-    <t>revFullName</t>
-  </si>
-  <si>
-    <t>dateRev</t>
-  </si>
-  <si>
-    <t>revIDby</t>
-  </si>
-  <si>
-    <t>Harvey Janszen</t>
-  </si>
-  <si>
-    <t>vElev</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>idDate</t>
-  </si>
-  <si>
-    <t>idBy</t>
-  </si>
-  <si>
     <t>vlat</t>
   </si>
   <si>
     <t>vlon</t>
   </si>
   <si>
-    <t>recordedBy</t>
+    <t>V078911</t>
+  </si>
+  <si>
+    <t>V083201</t>
+  </si>
+  <si>
+    <t>roadside and meadow; common</t>
+  </si>
+  <si>
+    <t>Mayne Island</t>
+  </si>
+  <si>
+    <t>V083236</t>
+  </si>
+  <si>
+    <t>abandoned farm fields</t>
+  </si>
+  <si>
+    <t>V083305</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Achillea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">millefolium </t>
+  </si>
+  <si>
+    <t>authority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L. </t>
+  </si>
+  <si>
+    <t>L.</t>
+  </si>
+  <si>
+    <t>Daucus</t>
+  </si>
+  <si>
+    <t>carota</t>
+  </si>
+  <si>
+    <t>Allium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vineale </t>
+  </si>
+  <si>
+    <t>(Nutt.) Coulter &amp; Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lomatium </t>
+  </si>
+  <si>
+    <t>utriculatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allium </t>
+  </si>
+  <si>
+    <t>cernuum</t>
+  </si>
+  <si>
+    <t>Roth</t>
+  </si>
+  <si>
+    <t>dry ridge</t>
+  </si>
+  <si>
+    <t>acuminatum</t>
+  </si>
+  <si>
+    <t>Hook.</t>
+  </si>
+  <si>
+    <t>Mayne Island; Mount Parke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,12 +186,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,99 +525,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8F860-94CC-D344-8430-EBA5B904AFFA}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="9" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="2" max="3" width="17" customWidth="1"/>
+    <col min="4" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3">
+        <v>48</v>
+      </c>
+      <c r="H3" s="3">
+        <v>123</v>
+      </c>
+      <c r="I3" s="4">
+        <v>27610</v>
+      </c>
+      <c r="J3" s="3">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="G4" s="3">
+        <v>48</v>
+      </c>
+      <c r="H4" s="3">
+        <v>123</v>
+      </c>
+      <c r="I4" s="4">
+        <v>27584</v>
+      </c>
+      <c r="J4" s="3">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2">
-        <v>115</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3">
+        <v>48</v>
+      </c>
+      <c r="H5" s="3">
+        <v>123</v>
+      </c>
+      <c r="I5" s="4">
+        <v>27544</v>
+      </c>
+      <c r="J5" s="3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>83309</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>48</v>
+      </c>
+      <c r="H6" s="3">
+        <v>123</v>
+      </c>
+      <c r="I6" s="4">
+        <v>27583</v>
+      </c>
+      <c r="J6" s="3">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>83310</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="3">
+        <v>48</v>
+      </c>
+      <c r="H7" s="3">
+        <v>123</v>
+      </c>
+      <c r="I7" s="4">
+        <v>27583</v>
+      </c>
+      <c r="J7" s="3">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>